<commit_message>
evaluation and paper updated
</commit_message>
<xml_diff>
--- a/Code/AgenticAdr.xlsx
+++ b/Code/AgenticAdr.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="147">
   <si>
     <t>Timestamp</t>
   </si>
@@ -271,6 +271,42 @@
     <t xml:space="preserve">I liked these, these are straight to the point and clear and crisp. Context and Decision is super linked and relevant to the codebase. </t>
   </si>
   <si>
+    <t>Bassam</t>
+  </si>
+  <si>
+    <t>mailbasam@gmail.com</t>
+  </si>
+  <si>
+    <t>https://github.com/pgexporter/pgexporter</t>
+  </si>
+  <si>
+    <t>Pretty good, it missed out details about bridge, compressions, extension support metrics</t>
+  </si>
+  <si>
+    <t>mentioned about the in-house  wire-protocol instead of library include. much more points covered for eg bridge, extensions, versioning etc. A little too small ADRs though.</t>
+  </si>
+  <si>
+    <t>too much focus on embedded things while omitting alot of other important things covered in the dir2.</t>
+  </si>
+  <si>
+    <t>covered almost all facets, but there is a lack of depth to each.</t>
+  </si>
+  <si>
+    <t>https://github.com/sudokara/SpecFlow</t>
+  </si>
+  <si>
+    <t>Context and decision have observations about the codebase (sometimes specific files/packages, which can be renamed/removed). The consequences are too wordy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context is only observations from codebase. Too many ADRs generated, not architecturally relevant. A lot of ADRs seem to come from observations done on requirements.txt, config.toml and other setup helpers. Consequences are concise and to the point </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consequences could have been split into pros and cons. Context and decision well captured. Most ADRs are well done. Some face similar issues as other ones, ie inferring only from requirements.txt and making comments on specific files that exist. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Context and decision are too vague and short. Too many ADRs generated, many are about roles of specific files in the codebase. Consequences could have been split into pros and cons. </t>
+  </si>
+  <si>
     <t>Is it your repository?</t>
   </si>
   <si>
@@ -376,9 +412,6 @@
     <t>https://github.com/sudokara/bracket</t>
   </si>
   <si>
-    <t>https://github.com/sudokara/SpecFlow</t>
-  </si>
-  <si>
     <t>https://github.com/microsoft/sarathi-serve</t>
   </si>
   <si>
@@ -455,6 +488,12 @@
   </si>
   <si>
     <t>https://github.com/ShailenderGoyal/PageRank-Algorithm</t>
+  </si>
+  <si>
+    <t>Bassam Adnan</t>
+  </si>
+  <si>
+    <t>mailbassam@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -464,7 +503,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -501,11 +540,6 @@
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -515,7 +549,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border/>
     <border>
       <left style="thin">
@@ -685,53 +719,11 @@
         <color rgb="FF442F65"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF442F65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF8F9FA"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF8F9FA"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF442F65"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -804,18 +796,6 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -860,15 +840,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle count="3" pivot="0" name="Form Responses 2-style">
+    <tableStyle count="4" pivot="0" name="Form Responses 2-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement size="0" type="wholeTable"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="Form Responses 1-style">
+    <tableStyle count="4" pivot="0" name="Form Responses 1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement size="0" type="wholeTable"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -883,7 +865,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:AC10" displayName="Form_Responses2" name="Form_Responses2" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:AC12" displayName="Form_Responses2" name="Form_Responses2" id="1">
   <tableColumns count="29">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -925,7 +907,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E45" displayName="Form_Responses" name="Form_Responses" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E46" displayName="Form_Responses" name="Form_Responses" id="2">
   <tableColumns count="5">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Name" id="2"/>
@@ -1975,92 +1957,270 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16">
+      <c r="A10" s="12">
         <v>45946.65276008102</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="13">
         <v>2.0</v>
       </c>
-      <c r="F10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="G10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="H10" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="I10" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="J10" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="K10" s="17" t="s">
+      <c r="F10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="G10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="H10" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="J10" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="K10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="M10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="N10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="O10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="P10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="Q10" s="17" t="s">
+      <c r="L10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="M10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="N10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="O10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="P10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="Q10" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="R10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="S10" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="T10" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="U10" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="V10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="W10" s="17" t="s">
+      <c r="R10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="S10" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="T10" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="U10" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="V10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="W10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="X10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="Y10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="Z10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="AA10" s="17">
-        <v>5.0</v>
-      </c>
-      <c r="AB10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="AC10" s="19" t="s">
+      <c r="X10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="Y10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="Z10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="AA10" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="AB10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="AC10" s="15" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8">
+        <v>45946.97044625</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="M11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="N11" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="P11" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R11" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="S11" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="T11" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="U11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="V11" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="X11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="Y11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="Z11" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="AC11" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="16">
+        <v>45947.74719896991</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="G12" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="H12" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="I12" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="M12" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="N12" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="O12" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="P12" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="Q12" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="R12" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="S12" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="T12" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="U12" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="V12" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="W12" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="X12" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="Y12" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="Z12" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="AA12" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="AB12" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="AC12" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2074,10 +2234,12 @@
     <hyperlink r:id="rId7" ref="D8"/>
     <hyperlink r:id="rId8" ref="D9"/>
     <hyperlink r:id="rId9" ref="D10"/>
+    <hyperlink r:id="rId10" ref="D11"/>
+    <hyperlink r:id="rId11" ref="D12"/>
   </hyperlinks>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2116,7 +2278,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
@@ -2133,7 +2295,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
@@ -2141,16 +2303,16 @@
         <v>45935.6874683912</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
@@ -2158,16 +2320,16 @@
         <v>45935.68841295139</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -2181,10 +2343,10 @@
         <v>66</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
@@ -2201,7 +2363,7 @@
         <v>67</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
@@ -2209,16 +2371,16 @@
         <v>45939.398966747685</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8">
@@ -2226,16 +2388,16 @@
         <v>45939.39946393519</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9">
@@ -2243,16 +2405,16 @@
         <v>45939.42655188657</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
@@ -2260,16 +2422,16 @@
         <v>45939.46848215278</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
@@ -2277,16 +2439,16 @@
         <v>45939.46881931713</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12">
@@ -2294,16 +2456,16 @@
         <v>45939.46913090278</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
@@ -2311,16 +2473,16 @@
         <v>45939.469453136575</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14">
@@ -2328,16 +2490,16 @@
         <v>45939.47011765046</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
@@ -2345,16 +2507,16 @@
         <v>45939.47123679398</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
@@ -2362,16 +2524,16 @@
         <v>45939.4715616551</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17">
@@ -2379,16 +2541,16 @@
         <v>45939.4719315625</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18">
@@ -2405,7 +2567,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
@@ -2416,13 +2578,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
@@ -2439,7 +2601,7 @@
         <v>27</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
@@ -2456,7 +2618,7 @@
         <v>41</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22">
@@ -2473,7 +2635,7 @@
         <v>53</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23">
@@ -2490,7 +2652,7 @@
         <v>48</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24">
@@ -2498,16 +2660,16 @@
         <v>45943.77945240741</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25">
@@ -2515,16 +2677,16 @@
         <v>45943.78019240741</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26">
@@ -2532,16 +2694,16 @@
         <v>45943.80242072917</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27">
@@ -2558,7 +2720,7 @@
         <v>60</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28">
@@ -2572,10 +2734,10 @@
         <v>59</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29">
@@ -2589,10 +2751,10 @@
         <v>59</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30">
@@ -2606,10 +2768,10 @@
         <v>59</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31">
@@ -2617,16 +2779,16 @@
         <v>45943.81834320602</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32">
@@ -2634,16 +2796,16 @@
         <v>45943.81866615741</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33">
@@ -2651,16 +2813,16 @@
         <v>45943.819046770834</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34">
@@ -2668,16 +2830,16 @@
         <v>45943.81948928241</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35">
@@ -2685,16 +2847,16 @@
         <v>45943.819892604166</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36">
@@ -2702,16 +2864,16 @@
         <v>45943.82017013889</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37">
@@ -2719,16 +2881,16 @@
         <v>45943.820890856485</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38">
@@ -2736,16 +2898,16 @@
         <v>45943.88293743056</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39">
@@ -2753,16 +2915,16 @@
         <v>45944.39525381944</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40">
@@ -2779,7 +2941,7 @@
         <v>34</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41">
@@ -2787,16 +2949,16 @@
         <v>45944.88423947917</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42">
@@ -2804,16 +2966,16 @@
         <v>45945.5456787963</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43">
@@ -2821,16 +2983,16 @@
         <v>45946.02685496528</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44">
@@ -2838,33 +3000,50 @@
         <v>45946.029433668984</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="24">
+      <c r="A45" s="8">
         <v>45946.03070726852</v>
       </c>
-      <c r="B45" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>73</v>
+      <c r="B45" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="16">
+        <v>45946.749427523144</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2913,10 +3092,11 @@
     <hyperlink r:id="rId42" ref="D43"/>
     <hyperlink r:id="rId43" ref="D44"/>
     <hyperlink r:id="rId44" ref="D45"/>
+    <hyperlink r:id="rId45" ref="D46"/>
   </hyperlinks>
-  <drawing r:id="rId45"/>
+  <drawing r:id="rId46"/>
   <tableParts count="1">
-    <tablePart r:id="rId47"/>
+    <tablePart r:id="rId48"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>